<commit_message>
add feature: type of tests
</commit_message>
<xml_diff>
--- a/test-data.xlsx
+++ b/test-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="73">
   <si>
     <t xml:space="preserve">Produit</t>
   </si>
@@ -49,6 +49,18 @@
     <t xml:space="preserve">full z</t>
   </si>
   <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">réalisé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validé</t>
+  </si>
+  <si>
     <t xml:space="preserve">P0001</t>
   </si>
   <si>
@@ -67,6 +79,9 @@
     <t xml:space="preserve">oui</t>
   </si>
   <si>
+    <t xml:space="preserve">reconstruction</t>
+  </si>
+  <si>
     <t xml:space="preserve">P0002</t>
   </si>
   <si>
@@ -218,6 +233,12 @@
   </si>
   <si>
     <t xml:space="preserve">S0018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restauration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resynchro</t>
   </si>
 </sst>
 </file>
@@ -293,12 +314,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -491,10 +516,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M40" activeCellId="0" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -527,468 +552,1246 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>18</v>
+      <c r="C35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
manage squad without colors defined
</commit_message>
<xml_diff>
--- a/test-data.xlsx
+++ b/test-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="87">
   <si>
     <t xml:space="preserve">Produit</t>
   </si>
@@ -239,6 +239,48 @@
   </si>
   <si>
     <t xml:space="preserve">resynchro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S0019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">squad inconnue 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P6666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S6666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribue 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">squad inconnue 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S6667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">squad inconnue 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S6668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">squad inconnue 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S6669</t>
+  </si>
+  <si>
+    <t xml:space="preserve">squad inconnue 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S6670</t>
+  </si>
+  <si>
+    <t xml:space="preserve">squad inconnue 6</t>
   </si>
 </sst>
 </file>
@@ -314,16 +356,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -516,10 +554,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M40" activeCellId="0" sqref="M40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -552,16 +590,16 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -590,13 +628,13 @@
       <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -625,10 +663,10 @@
       <c r="H3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -657,7 +695,7 @@
       <c r="I4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -683,13 +721,13 @@
       <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="2" t="s">
+      <c r="K5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -718,7 +756,7 @@
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -747,7 +785,7 @@
       <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -776,10 +814,10 @@
       <c r="H8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -808,13 +846,13 @@
       <c r="H9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="2" t="s">
+      <c r="K9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -843,10 +881,10 @@
       <c r="H10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -875,7 +913,7 @@
       <c r="H11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -904,10 +942,10 @@
       <c r="H12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -936,7 +974,7 @@
       <c r="H13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -965,7 +1003,7 @@
       <c r="H14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -994,10 +1032,10 @@
       <c r="H15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1024,10 +1062,10 @@
       <c r="H16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1056,7 +1094,7 @@
       <c r="H17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1085,10 +1123,10 @@
       <c r="H18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1117,10 +1155,10 @@
       <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="M19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1149,7 +1187,7 @@
       <c r="H20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1178,13 +1216,13 @@
       <c r="H21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L21" s="2" t="s">
+      <c r="K21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1213,7 +1251,7 @@
       <c r="I22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1239,7 +1277,7 @@
       <c r="H23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1268,10 +1306,10 @@
       <c r="H24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="M24" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1300,7 +1338,7 @@
       <c r="I25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1329,7 +1367,7 @@
       <c r="H26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1358,10 +1396,10 @@
       <c r="H27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="L27" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1390,10 +1428,10 @@
       <c r="H28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="M28" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1422,10 +1460,10 @@
       <c r="H29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="J29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="K29" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1454,10 +1492,10 @@
       <c r="H30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="L30" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1486,7 +1524,7 @@
       <c r="H31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J31" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1515,7 +1553,7 @@
       <c r="H32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1544,10 +1582,10 @@
       <c r="H33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="J33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="M33" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1574,7 +1612,7 @@
       <c r="H34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1603,7 +1641,7 @@
       <c r="H35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1632,10 +1670,10 @@
       <c r="H36" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J36" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="L36" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1664,10 +1702,10 @@
       <c r="H37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J37" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M37" s="2" t="s">
+      <c r="M37" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1694,10 +1732,10 @@
       <c r="H38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="K38" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1726,10 +1764,10 @@
       <c r="H39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="L39" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1758,10 +1796,10 @@
       <c r="H40" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J40" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="K40" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1770,7 +1808,7 @@
         <v>69</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>54</v>
@@ -1779,7 +1817,7 @@
         <v>58</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>18</v>
@@ -1790,7 +1828,152 @@
       <c r="H41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J46" s="1" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some fix about stats
</commit_message>
<xml_diff>
--- a/test-data.xlsx
+++ b/test-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="88">
   <si>
     <t xml:space="preserve">Produit</t>
   </si>
@@ -238,7 +238,7 @@
     <t xml:space="preserve">restauration</t>
   </si>
   <si>
-    <t xml:space="preserve">resynchro</t>
+    <t xml:space="preserve">resynchronisation</t>
   </si>
   <si>
     <t xml:space="preserve">S0019</t>
@@ -281,6 +281,9 @@
   </si>
   <si>
     <t xml:space="preserve">squad inconnue 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restauration bdd</t>
   </si>
 </sst>
 </file>
@@ -356,12 +359,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -554,10 +561,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="1" sqref="D1:D46 B42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F47" activeCellId="0" sqref="F47:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1860,6 +1867,9 @@
       <c r="J42" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="K42" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
@@ -1889,6 +1899,9 @@
       <c r="J43" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="K43" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
@@ -1918,6 +1931,9 @@
       <c r="J44" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="K44" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
@@ -1975,6 +1991,29 @@
       </c>
       <c r="J46" s="1" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="J47" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>